<commit_message>
update table and diagrams of results
</commit_message>
<xml_diff>
--- a/Experiment results/results and diagrams for paper.xlsx
+++ b/Experiment results/results and diagrams for paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03C5E231-6D0E-458D-A081-2FF9B696F9DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03345C-D38F-4A64-BF3D-0687F23BE731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA2EA969-788C-49C5-B342-48FDE6047D9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>Class</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Robinson</t>
+  </si>
+  <si>
+    <t>Map Identification</t>
+  </si>
+  <si>
+    <t>Non-map</t>
+  </si>
+  <si>
+    <t>Map</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -169,13 +178,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -981,7 +996,590 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$27:$B$34</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Non-map</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Map</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>96.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B6C-4DE6-9F5D-AA4B487EE14F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recall (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$27:$B$34</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Non-map</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Map</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$27:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>93.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B6C-4DE6-9F5D-AA4B487EE14F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1 Score (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$27:$B$34</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Non-map</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Map</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>94.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B6C-4DE6-9F5D-AA4B487EE14F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1586607856"/>
+        <c:axId val="1355600416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1586607856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355600416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1355600416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="84"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1586607856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1524,6 +2122,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1557,6 +2658,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>175441</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>31025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>480241</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>150768</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3A959A4-C15C-47C8-8D45-BBA97053A1F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1862,10 +2999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC72171-B520-49C3-8F54-6B93B34737C5}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1900,7 +3037,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1962,7 +3099,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1979,7 +3116,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1994,7 +3131,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2009,7 +3146,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2024,7 +3161,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2041,7 +3178,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -2056,7 +3193,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -2071,7 +3208,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2086,7 +3223,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2103,7 +3240,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -2118,7 +3255,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2133,7 +3270,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2148,7 +3285,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2165,7 +3302,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +3317,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2195,7 +3332,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="6"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2209,8 +3346,157 @@
         <v>94.9</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>96.9</v>
+      </c>
+      <c r="D27" s="4">
+        <v>93.1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
+      <c r="B28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="4">
+        <v>91.7</v>
+      </c>
+      <c r="D28" s="4">
+        <v>91.7</v>
+      </c>
+      <c r="E28" s="4">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="4">
+        <v>96.9</v>
+      </c>
+      <c r="D29" s="4">
+        <v>94</v>
+      </c>
+      <c r="E29" s="4">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4">
+        <v>98.1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>99.1</v>
+      </c>
+      <c r="E30" s="4">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="4">
+        <v>93.2</v>
+      </c>
+      <c r="D31" s="4">
+        <v>97</v>
+      </c>
+      <c r="E31" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="8"/>
+      <c r="B32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="4">
+        <v>90.2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>90.2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="8"/>
+      <c r="B33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="4">
+        <v>94.2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>97</v>
+      </c>
+      <c r="E33" s="4">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="9"/>
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="5">
+        <v>98.9</v>
+      </c>
+      <c r="D34" s="5">
+        <v>97.9</v>
+      </c>
+      <c r="E34" s="5">
+        <v>98.4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>

</xml_diff>

<commit_message>
update MLP results for batch size testing
</commit_message>
<xml_diff>
--- a/Experiment results/results and diagrams for paper.xlsx
+++ b/Experiment results/results and diagrams for paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03345C-D38F-4A64-BF3D-0687F23BE731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20681634-7C9A-407D-ABF9-0E9199F77F2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA2EA969-788C-49C5-B342-48FDE6047D9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Class</t>
   </si>
@@ -87,6 +87,27 @@
   </si>
   <si>
     <t>Map</t>
+  </si>
+  <si>
+    <t>Training size test</t>
+  </si>
+  <si>
+    <t>Training Size</t>
+  </si>
+  <si>
+    <t>Testing Accuracy Rate (%)</t>
+  </si>
+  <si>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>CNN (from scratch)</t>
+  </si>
+  <si>
+    <t>CNN (transfer learning)</t>
   </si>
 </sst>
 </file>
@@ -164,9 +185,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -184,13 +211,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1539,6 +1566,833 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Testing Accuracy Rate (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-55AA-42AA-A72F-612223329634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$62:$B$77</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>800</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$62:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>98.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-55AA-42AA-A72F-612223329634}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$62:$B$77</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>800</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-55AA-42AA-A72F-612223329634}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="1268836047"/>
+        <c:axId val="1280995967"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$62:$B$77</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>800</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>200</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>400</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>600</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>800</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-55AA-42AA-A72F-612223329634}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1268836047"/>
+        <c:axId val="1280995967"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1268836047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280995967"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280995967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1268836047"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1619,6 +2473,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2123,6 +3017,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2694,6 +4091,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>125186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B183D39C-71E6-4880-9D9C-67F4CBF72C38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2999,10 +4432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC72171-B520-49C3-8F54-6B93B34737C5}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3037,7 +4470,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3054,7 +4487,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3069,7 +4502,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -3084,7 +4517,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3099,7 +4532,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3116,7 +4549,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -3131,7 +4564,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -3146,7 +4579,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -3161,7 +4594,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3178,7 +4611,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -3193,7 +4626,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -3208,7 +4641,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -3223,7 +4656,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3240,7 +4673,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -3255,7 +4688,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -3270,7 +4703,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -3285,7 +4718,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3302,7 +4735,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -3317,7 +4750,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3332,7 +4765,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -3370,7 +4803,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -3387,7 +4820,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
@@ -3402,7 +4835,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
@@ -3417,7 +4850,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="4" t="s">
         <v>8</v>
       </c>
@@ -3432,7 +4865,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -3449,7 +4882,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
@@ -3464,7 +4897,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
@@ -3479,7 +4912,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -3493,8 +4926,382 @@
         <v>98.4</v>
       </c>
     </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="6">
+        <v>200</v>
+      </c>
+      <c r="C39" s="6">
+        <v>87</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="9"/>
+      <c r="B40" s="6">
+        <v>400</v>
+      </c>
+      <c r="C40" s="6">
+        <v>90.5</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="6">
+        <v>600</v>
+      </c>
+      <c r="C41" s="6">
+        <v>90.4</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="9"/>
+      <c r="B42" s="6">
+        <v>800</v>
+      </c>
+      <c r="C42" s="6">
+        <v>95</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="6">
+        <v>200</v>
+      </c>
+      <c r="C43" s="6">
+        <v>87.5</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="9"/>
+      <c r="B44" s="6">
+        <v>400</v>
+      </c>
+      <c r="C44" s="6">
+        <v>89.5</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="9"/>
+      <c r="B45" s="6">
+        <v>600</v>
+      </c>
+      <c r="C45" s="6">
+        <v>90</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="9"/>
+      <c r="B46" s="6">
+        <v>800</v>
+      </c>
+      <c r="C46" s="6">
+        <v>91</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="6">
+        <v>200</v>
+      </c>
+      <c r="C47" s="6">
+        <v>90.5</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="9"/>
+      <c r="B48" s="6">
+        <v>400</v>
+      </c>
+      <c r="C48" s="6">
+        <v>93</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="9"/>
+      <c r="B49" s="6">
+        <v>600</v>
+      </c>
+      <c r="C49" s="6">
+        <v>93</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="9"/>
+      <c r="B50" s="6">
+        <v>800</v>
+      </c>
+      <c r="C50" s="6">
+        <v>95.5</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="6">
+        <v>200</v>
+      </c>
+      <c r="C51" s="6">
+        <v>96</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="9"/>
+      <c r="B52" s="6">
+        <v>400</v>
+      </c>
+      <c r="C52" s="6">
+        <v>97</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+    </row>
+    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="9"/>
+      <c r="B53" s="6">
+        <v>600</v>
+      </c>
+      <c r="C53" s="6">
+        <v>97.5</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+    </row>
+    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="10"/>
+      <c r="B54" s="7">
+        <v>800</v>
+      </c>
+      <c r="C54" s="7">
+        <v>98.5</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+    </row>
+    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="1:5" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="6">
+        <v>200</v>
+      </c>
+      <c r="C62" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="11"/>
+      <c r="B63" s="6">
+        <v>400</v>
+      </c>
+      <c r="C63" s="6">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="11"/>
+      <c r="B64" s="6">
+        <v>600</v>
+      </c>
+      <c r="C64" s="6">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="11"/>
+      <c r="B65" s="7">
+        <v>800</v>
+      </c>
+      <c r="C65" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="6">
+        <v>200</v>
+      </c>
+      <c r="C66" s="6">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="9"/>
+      <c r="B67" s="6">
+        <v>400</v>
+      </c>
+      <c r="C67" s="6">
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="9"/>
+      <c r="B68" s="6">
+        <v>600</v>
+      </c>
+      <c r="C68" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="9"/>
+      <c r="B69" s="7">
+        <v>800</v>
+      </c>
+      <c r="C69" s="6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="6">
+        <v>200</v>
+      </c>
+      <c r="C70" s="6">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="9"/>
+      <c r="B71" s="6">
+        <v>400</v>
+      </c>
+      <c r="C71" s="6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="9"/>
+      <c r="B72" s="6">
+        <v>600</v>
+      </c>
+      <c r="C72" s="6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="9"/>
+      <c r="B73" s="7">
+        <v>800</v>
+      </c>
+      <c r="C73" s="6">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="6">
+        <v>200</v>
+      </c>
+      <c r="C74" s="6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="9"/>
+      <c r="B75" s="6">
+        <v>400</v>
+      </c>
+      <c r="C75" s="6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="9"/>
+      <c r="B76" s="6">
+        <v>600</v>
+      </c>
+      <c r="C76" s="6">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="9"/>
+      <c r="B77" s="7">
+        <v>800</v>
+      </c>
+      <c r="C77" s="7">
+        <v>98.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="15">
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A62:A65"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A3:A6"/>

</xml_diff>

<commit_message>
update CNN code for shifted maps
</commit_message>
<xml_diff>
--- a/Experiment results/results and diagrams for paper.xlsx
+++ b/Experiment results/results and diagrams for paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20681634-7C9A-407D-ABF9-0E9199F77F2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEB0F2F-C184-4777-8FFD-AB02DB9248F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA2EA969-788C-49C5-B342-48FDE6047D9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="20">
   <si>
     <t>Class</t>
   </si>
@@ -92,22 +92,7 @@
     <t>Training size test</t>
   </si>
   <si>
-    <t>Training Size</t>
-  </si>
-  <si>
     <t>Testing Accuracy Rate (%)</t>
-  </si>
-  <si>
-    <t>MLP</t>
-  </si>
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>CNN (from scratch)</t>
-  </si>
-  <si>
-    <t>CNN (transfer learning)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,6 +197,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1592,7 +1586,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$61</c:f>
+              <c:f>Sheet1!$C$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1841,7 +1835,7 @@
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$62:$B$77</c:f>
+              <c:f>Sheet1!$A$43:$B$58</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1913,7 +1907,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$C$77</c:f>
+              <c:f>Sheet1!$C$43:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2000,7 +1994,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$62:$B$77</c:f>
+              <c:f>Sheet1!$A$43:$B$58</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -2131,7 +2125,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$62:$B$77</c:f>
+              <c:f>Sheet1!$A$43:$B$58</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -2393,6 +2387,794 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$62:$B$76</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$62:$C$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>91.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>98.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$62:$B$76</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$62:$B$76</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>50</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8EA8-40A3-A1EA-D7BE948B12F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="490296048"/>
+        <c:axId val="486077152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="490296048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="486077152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="486077152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="490296048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2513,6 +3295,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3520,6 +4342,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4100,13 +5425,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>348343</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>125186</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>43543</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>70757</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4127,6 +5452,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7EAB8F7-35E2-44D6-B441-B405DCE4C1A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4432,10 +5793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC72171-B520-49C3-8F54-6B93B34737C5}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4470,7 +5831,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4487,7 +5848,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -4502,7 +5863,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4517,7 +5878,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4532,7 +5893,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -4549,7 +5910,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -4564,7 +5925,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -4579,7 +5940,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -4594,7 +5955,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4611,7 +5972,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -4626,7 +5987,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -4641,7 +6002,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -4656,7 +6017,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4673,7 +6034,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -4688,7 +6049,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -4703,7 +6064,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -4718,7 +6079,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -4735,7 +6096,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -4750,7 +6111,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4765,7 +6126,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="10"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4803,7 +6164,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -4820,7 +6181,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +6196,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
@@ -4850,7 +6211,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="4" t="s">
         <v>8</v>
       </c>
@@ -4865,7 +6226,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -4882,7 +6243,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
@@ -4897,7 +6258,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
@@ -4912,7 +6273,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="10"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -4926,210 +6287,177 @@
         <v>98.4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="1:5" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="6">
-        <v>200</v>
-      </c>
-      <c r="C39" s="6">
-        <v>87</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
-      <c r="B40" s="6">
-        <v>400</v>
-      </c>
-      <c r="C40" s="6">
-        <v>90.5</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="6">
-        <v>600</v>
-      </c>
-      <c r="C41" s="6">
-        <v>90.4</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
-      <c r="B42" s="6">
-        <v>800</v>
-      </c>
-      <c r="C42" s="6">
-        <v>95</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="9" t="s">
-        <v>22</v>
+      <c r="A43" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="B43" s="6">
         <v>200</v>
       </c>
       <c r="C43" s="6">
-        <v>87.5</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="6">
         <v>400</v>
       </c>
       <c r="C44" s="6">
-        <v>89.5</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+        <v>90.5</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="6">
         <v>600</v>
       </c>
       <c r="C45" s="6">
-        <v>90</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+        <v>90.4</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="9"/>
-      <c r="B46" s="6">
+      <c r="A46" s="14"/>
+      <c r="B46" s="7">
         <v>800</v>
       </c>
       <c r="C46" s="6">
-        <v>91</v>
-      </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
+        <v>95</v>
+      </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="9" t="s">
-        <v>23</v>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B47" s="6">
         <v>200</v>
       </c>
       <c r="C47" s="6">
-        <v>90.5</v>
-      </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
+        <v>87.5</v>
+      </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="9"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="11"/>
       <c r="B48" s="6">
         <v>400</v>
       </c>
       <c r="C48" s="6">
-        <v>93</v>
-      </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+        <v>89.5</v>
+      </c>
     </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="9"/>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="11"/>
       <c r="B49" s="6">
         <v>600</v>
       </c>
       <c r="C49" s="6">
-        <v>93</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+        <v>90</v>
+      </c>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="9"/>
-      <c r="B50" s="6">
+    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="11"/>
+      <c r="B50" s="7">
         <v>800</v>
       </c>
       <c r="C50" s="6">
-        <v>95.5</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
+        <v>91</v>
+      </c>
     </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="9" t="s">
-        <v>24</v>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B51" s="6">
         <v>200</v>
       </c>
       <c r="C51" s="6">
-        <v>96</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
+        <v>90.5</v>
+      </c>
     </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="9"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="11"/>
       <c r="B52" s="6">
         <v>400</v>
       </c>
       <c r="C52" s="6">
-        <v>97</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
+        <v>93</v>
+      </c>
     </row>
-    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="9"/>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="11"/>
       <c r="B53" s="6">
         <v>600</v>
       </c>
       <c r="C53" s="6">
-        <v>97.5</v>
-      </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
+        <v>93</v>
+      </c>
     </row>
-    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="10"/>
+    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="11"/>
       <c r="B54" s="7">
         <v>800</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="6">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="6">
+        <v>200</v>
+      </c>
+      <c r="C55" s="6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="11"/>
+      <c r="B56" s="6">
+        <v>400</v>
+      </c>
+      <c r="C56" s="6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="11"/>
+      <c r="B57" s="6">
+        <v>600</v>
+      </c>
+      <c r="C57" s="6">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="11"/>
+      <c r="B58" s="7">
+        <v>800</v>
+      </c>
+      <c r="C58" s="7">
         <v>98.5</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="61" spans="1:5" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -5137,171 +6465,155 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="9">
+        <v>10</v>
+      </c>
+      <c r="C62" s="8">
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="14"/>
+      <c r="B63" s="9">
         <v>20</v>
       </c>
+      <c r="C63" s="9">
+        <v>95</v>
+      </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="6">
-        <v>200</v>
-      </c>
-      <c r="C62" s="6">
-        <v>87</v>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="14"/>
+      <c r="B64" s="9">
+        <v>30</v>
+      </c>
+      <c r="C64" s="9">
+        <v>92.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="11"/>
-      <c r="B63" s="6">
-        <v>400</v>
-      </c>
-      <c r="C63" s="6">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="11"/>
-      <c r="B64" s="6">
-        <v>600</v>
-      </c>
-      <c r="C64" s="6">
-        <v>90.4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="11"/>
-      <c r="B65" s="7">
-        <v>800</v>
-      </c>
-      <c r="C65" s="6">
-        <v>95</v>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="14"/>
+      <c r="B65" s="9">
+        <v>40</v>
+      </c>
+      <c r="C65" s="9">
+        <v>92.5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="6">
-        <v>200</v>
-      </c>
-      <c r="C66" s="6">
-        <v>87.5</v>
+      <c r="A66" s="14"/>
+      <c r="B66" s="9">
+        <v>50</v>
+      </c>
+      <c r="C66" s="9">
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="9"/>
-      <c r="B67" s="6">
-        <v>400</v>
-      </c>
-      <c r="C67" s="6">
-        <v>89.5</v>
+      <c r="A67" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="9">
+        <v>10</v>
+      </c>
+      <c r="C67" s="9">
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="9"/>
-      <c r="B68" s="6">
-        <v>600</v>
-      </c>
-      <c r="C68" s="6">
-        <v>90</v>
+      <c r="A68" s="11"/>
+      <c r="B68" s="9">
+        <v>20</v>
+      </c>
+      <c r="C68" s="9">
+        <v>95.5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="9"/>
-      <c r="B69" s="7">
-        <v>800</v>
-      </c>
-      <c r="C69" s="6">
-        <v>91</v>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="11"/>
+      <c r="B69" s="9">
+        <v>30</v>
+      </c>
+      <c r="C69" s="9">
+        <v>88.5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B70" s="6">
-        <v>200</v>
-      </c>
-      <c r="C70" s="6">
-        <v>90.5</v>
+      <c r="A70" s="11"/>
+      <c r="B70" s="9">
+        <v>40</v>
+      </c>
+      <c r="C70" s="9">
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="9"/>
-      <c r="B71" s="6">
-        <v>400</v>
-      </c>
-      <c r="C71" s="6">
-        <v>93</v>
+      <c r="A71" s="11"/>
+      <c r="B71" s="9">
+        <v>50</v>
+      </c>
+      <c r="C71" s="9">
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="9"/>
-      <c r="B72" s="6">
-        <v>600</v>
-      </c>
-      <c r="C72" s="6">
-        <v>93</v>
+      <c r="A72" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="9">
+        <v>10</v>
+      </c>
+      <c r="C72" s="9">
+        <v>98.5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="9"/>
-      <c r="B73" s="7">
-        <v>800</v>
-      </c>
-      <c r="C73" s="6">
-        <v>95.5</v>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="11"/>
+      <c r="B73" s="9">
+        <v>20</v>
+      </c>
+      <c r="C73" s="9">
+        <v>98.5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="6">
-        <v>200</v>
-      </c>
-      <c r="C74" s="6">
-        <v>96</v>
+      <c r="A74" s="11"/>
+      <c r="B74" s="9">
+        <v>30</v>
+      </c>
+      <c r="C74" s="9">
+        <v>98.5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="9"/>
-      <c r="B75" s="6">
-        <v>400</v>
-      </c>
-      <c r="C75" s="6">
-        <v>97</v>
+      <c r="A75" s="11"/>
+      <c r="B75" s="9">
+        <v>40</v>
+      </c>
+      <c r="C75" s="9">
+        <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="9"/>
-      <c r="B76" s="6">
-        <v>600</v>
-      </c>
-      <c r="C76" s="6">
-        <v>97.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="9"/>
-      <c r="B77" s="7">
-        <v>800</v>
-      </c>
-      <c r="C77" s="7">
+    <row r="76" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="11"/>
+      <c r="B76" s="9">
+        <v>50</v>
+      </c>
+      <c r="C76" s="10">
         <v>98.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A62:A65"/>
+  <mergeCells count="14">
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="A72:A76"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A3:A6"/>
@@ -5309,6 +6621,10 @@
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A43:A46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update MLP equalarea results
</commit_message>
<xml_diff>
--- a/Experiment results/results and diagrams for paper.xlsx
+++ b/Experiment results/results and diagrams for paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEB0F2F-C184-4777-8FFD-AB02DB9248F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884D5E19-3EC5-4F5F-9B7C-3DB4793EA825}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA2EA969-788C-49C5-B342-48FDE6047D9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
   <si>
     <t>Class</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Testing Accuracy Rate (%)</t>
+  </si>
+  <si>
+    <t>Batch size test</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -211,9 +214,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3175,6 +3188,688 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Testing Accuracy Rate (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-1B71-47C7-B55C-63B15A04B789}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$82:$B$93</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>180</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$82:$C$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B71-47C7-B55C-63B15A04B789}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$82:$B$93</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>180</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$82:$D$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1B71-47C7-B55C-63B15A04B789}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$82:$B$93</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>180</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>90</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>-90</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>180</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$82:$E$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1B71-47C7-B55C-63B15A04B789}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="685206032"/>
+        <c:axId val="689910464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="685206032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689910464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="689910464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="685206032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3335,6 +4030,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4845,6 +5580,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5488,6 +6726,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12156</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>316956</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{523124F9-1842-43C8-8CE9-2CB9F8BA4733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5793,10 +7067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC72171-B520-49C3-8F54-6B93B34737C5}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5831,7 +7105,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -5848,7 +7122,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -5863,7 +7137,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -5878,7 +7152,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -5893,7 +7167,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -5910,7 +7184,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -5925,7 +7199,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -5940,7 +7214,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -5955,7 +7229,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -5972,7 +7246,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -5987,7 +7261,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -6002,7 +7276,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -6017,7 +7291,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -6034,7 +7308,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -6049,7 +7323,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -6064,7 +7338,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -6079,7 +7353,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -6096,7 +7370,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -6111,7 +7385,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6126,7 +7400,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="13"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -6164,7 +7438,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -6181,7 +7455,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
@@ -6196,7 +7470,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
@@ -6211,7 +7485,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="4" t="s">
         <v>8</v>
       </c>
@@ -6226,7 +7500,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -6243,7 +7517,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="11"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
@@ -6258,7 +7532,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
@@ -6273,7 +7547,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="13"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -6305,7 +7579,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="6">
@@ -6316,7 +7590,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="6">
         <v>400</v>
       </c>
@@ -6325,7 +7599,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="6">
         <v>600</v>
       </c>
@@ -6334,7 +7608,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="7">
         <v>800</v>
       </c>
@@ -6343,7 +7617,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="6">
@@ -6354,7 +7628,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="11"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="6">
         <v>400</v>
       </c>
@@ -6363,7 +7637,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="11"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="6">
         <v>600</v>
       </c>
@@ -6372,7 +7646,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="11"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="7">
         <v>800</v>
       </c>
@@ -6381,7 +7655,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="6">
@@ -6392,7 +7666,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="11"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="6">
         <v>400</v>
       </c>
@@ -6401,7 +7675,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="11"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="6">
         <v>600</v>
       </c>
@@ -6410,7 +7684,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="11"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="7">
         <v>800</v>
       </c>
@@ -6419,7 +7693,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="6">
@@ -6430,7 +7704,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="11"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="6">
         <v>400</v>
       </c>
@@ -6439,7 +7713,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="11"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="6">
         <v>600</v>
       </c>
@@ -6448,7 +7722,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="11"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="7">
         <v>800</v>
       </c>
@@ -6456,7 +7730,11 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>0</v>
@@ -6469,7 +7747,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="9">
@@ -6480,7 +7758,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="14"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="9">
         <v>20</v>
       </c>
@@ -6489,7 +7767,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="14"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="9">
         <v>30</v>
       </c>
@@ -6498,7 +7776,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="14"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="9">
         <v>40</v>
       </c>
@@ -6507,7 +7785,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="14"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="9">
         <v>50</v>
       </c>
@@ -6516,7 +7794,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="9">
@@ -6527,7 +7805,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="11"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="9">
         <v>20</v>
       </c>
@@ -6536,7 +7814,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="11"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="9">
         <v>30</v>
       </c>
@@ -6545,7 +7823,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="11"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="9">
         <v>40</v>
       </c>
@@ -6554,7 +7832,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="11"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="9">
         <v>50</v>
       </c>
@@ -6563,7 +7841,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B72" s="9">
@@ -6574,7 +7852,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="11"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="9">
         <v>20</v>
       </c>
@@ -6583,7 +7861,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="11"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="9">
         <v>30</v>
       </c>
@@ -6592,7 +7870,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="11"/>
+      <c r="A75" s="16"/>
       <c r="B75" s="9">
         <v>40</v>
       </c>
@@ -6601,7 +7879,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="11"/>
+      <c r="A76" s="16"/>
       <c r="B76" s="9">
         <v>50</v>
       </c>
@@ -6609,18 +7887,176 @@
         <v>98.5</v>
       </c>
     </row>
+    <row r="80" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="12">
+        <v>90</v>
+      </c>
+      <c r="C82" s="12">
+        <v>97</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="15"/>
+      <c r="B83" s="11">
+        <v>-90</v>
+      </c>
+      <c r="C83" s="11">
+        <v>100</v>
+      </c>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+    </row>
+    <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="15"/>
+      <c r="B84" s="11">
+        <v>180</v>
+      </c>
+      <c r="C84" s="11">
+        <v>100</v>
+      </c>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="12">
+        <v>90</v>
+      </c>
+      <c r="C85" s="11">
+        <v>63.5</v>
+      </c>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="16"/>
+      <c r="B86" s="11">
+        <v>-90</v>
+      </c>
+      <c r="C86" s="11">
+        <v>54</v>
+      </c>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+    </row>
+    <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="16"/>
+      <c r="B87" s="11">
+        <v>180</v>
+      </c>
+      <c r="C87" s="11">
+        <v>44</v>
+      </c>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="12">
+        <v>90</v>
+      </c>
+      <c r="C88" s="11">
+        <v>100</v>
+      </c>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="16"/>
+      <c r="B89" s="11">
+        <v>-90</v>
+      </c>
+      <c r="C89" s="11">
+        <v>96.5</v>
+      </c>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+    </row>
+    <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="16"/>
+      <c r="B90" s="11">
+        <v>180</v>
+      </c>
+      <c r="C90" s="11">
+        <v>100</v>
+      </c>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="12">
+        <v>90</v>
+      </c>
+      <c r="C91" s="11">
+        <v>100</v>
+      </c>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="16"/>
+      <c r="B92" s="11">
+        <v>-90</v>
+      </c>
+      <c r="C92" s="11">
+        <v>100</v>
+      </c>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+    </row>
+    <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="16"/>
+      <c r="B93" s="11">
+        <v>180</v>
+      </c>
+      <c r="C93" s="13">
+        <v>100</v>
+      </c>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="18">
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A62:A66"/>
     <mergeCell ref="A67:A71"/>
     <mergeCell ref="A72:A76"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A55:A58"/>

</xml_diff>

<commit_message>
update MLP code for cea
</commit_message>
<xml_diff>
--- a/Experiment results/results and diagrams for paper.xlsx
+++ b/Experiment results/results and diagrams for paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884D5E19-3EC5-4F5F-9B7C-3DB4793EA825}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE85CE5-E75D-4AE9-BE0F-1E68EE74ADF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA2EA969-788C-49C5-B342-48FDE6047D9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
   <si>
     <t>Class</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>Batch size test</t>
+  </si>
+  <si>
+    <t>Shift testing</t>
+  </si>
+  <si>
+    <t>Other regions</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>The United States</t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
 </sst>
 </file>
@@ -173,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -214,6 +232,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -226,7 +251,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3870,6 +3894,790 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$101</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$102:$B$121</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Other regions</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>China</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>South Korea</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>The United States</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>World</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$102:$C$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>80.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>98.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>82.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>78.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>96.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B97-48EB-9B2F-FDBB7D0799B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$101</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recall (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$102:$B$121</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Other regions</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>China</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>South Korea</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>The United States</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>World</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$102:$D$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>79.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>97.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>98.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B97-48EB-9B2F-FDBB7D0799B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$101</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1 Score (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$102:$B$121</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Other regions</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>China</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>South Korea</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>The United States</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>World</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$102:$E$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>76.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>97.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>98.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>92.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>97.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B97-48EB-9B2F-FDBB7D0799B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="209039280"/>
+        <c:axId val="346693360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="209039280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346693360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="346693360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="209039280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4070,6 +4878,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6083,6 +6931,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6767,6 +8118,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>349612</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>6713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>139881</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DD4AB4-E7A9-4EF1-8886-602E9B59E5C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7067,10 +8454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC72171-B520-49C3-8F54-6B93B34737C5}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H120" sqref="H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7105,7 +8492,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -7122,7 +8509,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -7137,7 +8524,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -7152,7 +8539,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -7167,7 +8554,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -7184,7 +8571,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -7199,7 +8586,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -7214,7 +8601,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="16"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -7229,7 +8616,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -7246,7 +8633,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -7261,7 +8648,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -7276,7 +8663,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -7291,7 +8678,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -7308,7 +8695,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="16"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -7323,7 +8710,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -7338,7 +8725,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -7353,7 +8740,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -7370,7 +8757,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -7385,7 +8772,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -7400,7 +8787,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="17"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -7438,7 +8825,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -7455,7 +8842,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
@@ -7470,7 +8857,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="16"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
@@ -7485,7 +8872,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="16"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="4" t="s">
         <v>8</v>
       </c>
@@ -7500,7 +8887,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -7517,7 +8904,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="16"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
@@ -7532,7 +8919,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
@@ -7547,7 +8934,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="17"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -7579,7 +8966,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="6">
@@ -7590,7 +8977,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="15"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="6">
         <v>400</v>
       </c>
@@ -7599,7 +8986,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="15"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="6">
         <v>600</v>
       </c>
@@ -7608,7 +8995,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="15"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="7">
         <v>800</v>
       </c>
@@ -7617,7 +9004,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="6">
@@ -7628,7 +9015,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="16"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="6">
         <v>400</v>
       </c>
@@ -7637,7 +9024,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="16"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="6">
         <v>600</v>
       </c>
@@ -7646,7 +9033,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="16"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="7">
         <v>800</v>
       </c>
@@ -7655,7 +9042,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="6">
@@ -7666,7 +9053,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="16"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="6">
         <v>400</v>
       </c>
@@ -7675,7 +9062,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="16"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="6">
         <v>600</v>
       </c>
@@ -7684,7 +9071,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="16"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="7">
         <v>800</v>
       </c>
@@ -7693,7 +9080,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="6">
@@ -7704,7 +9091,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="16"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="6">
         <v>400</v>
       </c>
@@ -7713,7 +9100,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="16"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="6">
         <v>600</v>
       </c>
@@ -7722,7 +9109,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="16"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="7">
         <v>800</v>
       </c>
@@ -7747,7 +9134,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="9">
@@ -7758,7 +9145,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="9">
         <v>20</v>
       </c>
@@ -7767,7 +9154,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="15"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="9">
         <v>30</v>
       </c>
@@ -7776,7 +9163,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="9">
         <v>40</v>
       </c>
@@ -7785,7 +9172,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="15"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="9">
         <v>50</v>
       </c>
@@ -7794,7 +9181,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="9">
@@ -7805,7 +9192,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="16"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="9">
         <v>20</v>
       </c>
@@ -7814,7 +9201,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="16"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="9">
         <v>30</v>
       </c>
@@ -7823,7 +9210,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="16"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="9">
         <v>40</v>
       </c>
@@ -7832,7 +9219,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="16"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="9">
         <v>50</v>
       </c>
@@ -7841,7 +9228,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B72" s="9">
@@ -7852,7 +9239,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="16"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="9">
         <v>20</v>
       </c>
@@ -7861,7 +9248,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="16"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="9">
         <v>30</v>
       </c>
@@ -7870,7 +9257,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="16"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="9">
         <v>40</v>
       </c>
@@ -7879,7 +9266,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="16"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="9">
         <v>50</v>
       </c>
@@ -7887,7 +9274,11 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="80" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>0</v>
@@ -7895,14 +9286,14 @@
       <c r="B81" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="18" t="s">
+      <c r="C81" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B82" s="12">
@@ -7915,7 +9306,7 @@
       <c r="E82" s="11"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="15"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="11">
         <v>-90</v>
       </c>
@@ -7926,7 +9317,7 @@
       <c r="E83" s="11"/>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="15"/>
+      <c r="A84" s="18"/>
       <c r="B84" s="11">
         <v>180</v>
       </c>
@@ -7937,7 +9328,7 @@
       <c r="E84" s="11"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="16" t="s">
+      <c r="A85" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B85" s="12">
@@ -7950,7 +9341,7 @@
       <c r="E85" s="11"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="16"/>
+      <c r="A86" s="19"/>
       <c r="B86" s="11">
         <v>-90</v>
       </c>
@@ -7961,7 +9352,7 @@
       <c r="E86" s="11"/>
     </row>
     <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="16"/>
+      <c r="A87" s="19"/>
       <c r="B87" s="11">
         <v>180</v>
       </c>
@@ -7972,7 +9363,7 @@
       <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="16" t="s">
+      <c r="A88" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B88" s="12">
@@ -7985,7 +9376,7 @@
       <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="16"/>
+      <c r="A89" s="19"/>
       <c r="B89" s="11">
         <v>-90</v>
       </c>
@@ -7996,7 +9387,7 @@
       <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="16"/>
+      <c r="A90" s="19"/>
       <c r="B90" s="11">
         <v>180</v>
       </c>
@@ -8007,7 +9398,7 @@
       <c r="E90" s="11"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="16" t="s">
+      <c r="A91" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B91" s="12">
@@ -8020,7 +9411,7 @@
       <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="16"/>
+      <c r="A92" s="19"/>
       <c r="B92" s="11">
         <v>-90</v>
       </c>
@@ -8031,7 +9422,7 @@
       <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="16"/>
+      <c r="A93" s="19"/>
       <c r="B93" s="11">
         <v>180</v>
       </c>
@@ -8041,8 +9432,343 @@
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
     </row>
+    <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="14">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D102" s="14">
+        <v>72.5</v>
+      </c>
+      <c r="E102" s="14">
+        <v>76.3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" s="19"/>
+      <c r="B103" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" s="14">
+        <v>79.2</v>
+      </c>
+      <c r="D103" s="14">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="E103" s="14">
+        <v>77.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" s="19"/>
+      <c r="B104" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="14">
+        <v>78.8</v>
+      </c>
+      <c r="D104" s="14">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="E104" s="14">
+        <v>78.099999999999994</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="19"/>
+      <c r="B105" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" s="14">
+        <v>88.1</v>
+      </c>
+      <c r="D105" s="14">
+        <v>97.4</v>
+      </c>
+      <c r="E105" s="14">
+        <v>92.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="14">
+        <v>90.9</v>
+      </c>
+      <c r="D106" s="14">
+        <v>85.1</v>
+      </c>
+      <c r="E106" s="14">
+        <v>87.9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" s="19"/>
+      <c r="B107" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" s="14">
+        <v>88.6</v>
+      </c>
+      <c r="D107" s="14">
+        <v>84.8</v>
+      </c>
+      <c r="E107" s="14">
+        <v>86.7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" s="19"/>
+      <c r="B108" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="14">
+        <v>95.9</v>
+      </c>
+      <c r="D108" s="14">
+        <v>90.4</v>
+      </c>
+      <c r="E108" s="14">
+        <v>93.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="19"/>
+      <c r="B109" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="14">
+        <v>100</v>
+      </c>
+      <c r="D109" s="14">
+        <v>95</v>
+      </c>
+      <c r="E109" s="14">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="14">
+        <v>86.5</v>
+      </c>
+      <c r="D110" s="14">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="E110" s="14">
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" s="19"/>
+      <c r="B111" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C111" s="14">
+        <v>85.2</v>
+      </c>
+      <c r="D111" s="14">
+        <v>86.8</v>
+      </c>
+      <c r="E111" s="14">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="19"/>
+      <c r="B112" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="14">
+        <v>85.5</v>
+      </c>
+      <c r="D112" s="14">
+        <v>87</v>
+      </c>
+      <c r="E112" s="14">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" s="19"/>
+      <c r="B113" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="14">
+        <v>98.2</v>
+      </c>
+      <c r="D113" s="14">
+        <v>96.4</v>
+      </c>
+      <c r="E113" s="14">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="14">
+        <v>84.2</v>
+      </c>
+      <c r="D114" s="14">
+        <v>82.8</v>
+      </c>
+      <c r="E114" s="14">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" s="19"/>
+      <c r="B115" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" s="14">
+        <v>82.7</v>
+      </c>
+      <c r="D115" s="14">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E115" s="14">
+        <v>81.099999999999994</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" s="19"/>
+      <c r="B116" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="14">
+        <v>88.2</v>
+      </c>
+      <c r="D116" s="14">
+        <v>86.5</v>
+      </c>
+      <c r="E116" s="14">
+        <v>87.3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="19"/>
+      <c r="B117" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" s="14">
+        <v>100</v>
+      </c>
+      <c r="D117" s="14">
+        <v>96.2</v>
+      </c>
+      <c r="E117" s="14">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" s="14">
+        <v>78.7</v>
+      </c>
+      <c r="D118" s="14">
+        <v>98</v>
+      </c>
+      <c r="E118" s="14">
+        <v>87.3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="19"/>
+      <c r="B119" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="14">
+        <v>83</v>
+      </c>
+      <c r="D119" s="14">
+        <v>92.9</v>
+      </c>
+      <c r="E119" s="14">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" s="19"/>
+      <c r="B120" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="14">
+        <v>88.4</v>
+      </c>
+      <c r="D120" s="14">
+        <v>97.4</v>
+      </c>
+      <c r="E120" s="14">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="20"/>
+      <c r="B121" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="15">
+        <v>96.9</v>
+      </c>
+      <c r="D121" s="15">
+        <v>98.4</v>
+      </c>
+      <c r="E121" s="15">
+        <v>97.6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="23">
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="A110:A113"/>
     <mergeCell ref="A82:A84"/>
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="A88:A90"/>
@@ -8059,8 +9785,6 @@
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A43:A46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update CNN and SVM results for carto
</commit_message>
<xml_diff>
--- a/Experiment results/results and diagrams for paper.xlsx
+++ b/Experiment results/results and diagrams for paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE85CE5-E75D-4AE9-BE0F-1E68EE74ADF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD19D3B1-B07C-43C6-AD8F-B98370BEC137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA2EA969-788C-49C5-B342-48FDE6047D9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>Class</t>
   </si>
@@ -115,6 +115,12 @@
   <si>
     <t>World</t>
   </si>
+  <si>
+    <t>Equal-area projection</t>
+  </si>
+  <si>
+    <t>Nonequal-area projection</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,16 +245,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4592,6 +4604,547 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="209039280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$131</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$132:$B$139</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Nonequal-area projection</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Equal-area projection</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$132:$C$139</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1415-48E7-887B-598EB645F780}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$131</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recall (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$132:$B$139</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Nonequal-area projection</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Equal-area projection</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$132:$D$139</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1415-48E7-887B-598EB645F780}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$131</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1 Score (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$132:$B$139</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>M</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>CT</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Nonequal-area projection</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Equal-area projection</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$132:$E$139</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1415-48E7-887B-598EB645F780}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1566692479"/>
+        <c:axId val="1438741119"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1566692479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1438741119"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1438741119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1566692479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4918,6 +5471,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -7434,6 +8027,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8154,6 +9250,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>157843</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{218349FF-9C49-4E77-8479-AA726528979C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8454,10 +9586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC72171-B520-49C3-8F54-6B93B34737C5}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H120" sqref="H120"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8492,7 +9624,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -8509,7 +9641,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -8524,7 +9656,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -8539,7 +9671,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -8825,7 +9957,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -8966,7 +10098,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="6">
@@ -8977,7 +10109,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="18"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="6">
         <v>400</v>
       </c>
@@ -8986,7 +10118,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="18"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="6">
         <v>600</v>
       </c>
@@ -8995,7 +10127,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="18"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="7">
         <v>800</v>
       </c>
@@ -9134,7 +10266,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="9">
@@ -9145,7 +10277,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="18"/>
+      <c r="A63" s="22"/>
       <c r="B63" s="9">
         <v>20</v>
       </c>
@@ -9154,7 +10286,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="18"/>
+      <c r="A64" s="22"/>
       <c r="B64" s="9">
         <v>30</v>
       </c>
@@ -9163,7 +10295,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="18"/>
+      <c r="A65" s="22"/>
       <c r="B65" s="9">
         <v>40</v>
       </c>
@@ -9172,7 +10304,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="18"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="9">
         <v>50</v>
       </c>
@@ -9293,7 +10425,7 @@
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B82" s="12">
@@ -9306,7 +10438,7 @@
       <c r="E82" s="11"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="18"/>
+      <c r="A83" s="22"/>
       <c r="B83" s="11">
         <v>-90</v>
       </c>
@@ -9317,7 +10449,7 @@
       <c r="E83" s="11"/>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="18"/>
+      <c r="A84" s="22"/>
       <c r="B84" s="11">
         <v>180</v>
       </c>
@@ -9451,7 +10583,7 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="17" t="s">
+      <c r="A102" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B102" s="14" t="s">
@@ -9760,8 +10892,165 @@
         <v>97.6</v>
       </c>
     </row>
+    <row r="130" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B132" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" s="17">
+        <v>98.5</v>
+      </c>
+      <c r="D132" s="17">
+        <v>98.5</v>
+      </c>
+      <c r="E132" s="17">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" s="19"/>
+      <c r="B133" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133" s="17">
+        <v>96.4</v>
+      </c>
+      <c r="D133" s="17">
+        <v>98.9</v>
+      </c>
+      <c r="E133" s="17">
+        <v>97.6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" s="19"/>
+      <c r="B134" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" s="17">
+        <v>98.6</v>
+      </c>
+      <c r="D134" s="17">
+        <v>100</v>
+      </c>
+      <c r="E134" s="17">
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" s="19"/>
+      <c r="B135" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135" s="17">
+        <v>100</v>
+      </c>
+      <c r="D135" s="17">
+        <v>100</v>
+      </c>
+      <c r="E135" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136" s="17">
+        <v>93.9</v>
+      </c>
+      <c r="D136" s="17">
+        <v>93.9</v>
+      </c>
+      <c r="E136" s="17">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" s="19"/>
+      <c r="B137" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137" s="17">
+        <v>96.5</v>
+      </c>
+      <c r="D137" s="17">
+        <v>88.7</v>
+      </c>
+      <c r="E137" s="17">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" s="19"/>
+      <c r="B138" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138" s="17">
+        <v>100</v>
+      </c>
+      <c r="D138" s="17">
+        <v>93</v>
+      </c>
+      <c r="E138" s="17">
+        <v>96.4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A139" s="20"/>
+      <c r="B139" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="18">
+        <v>100</v>
+      </c>
+      <c r="D139" s="18">
+        <v>100</v>
+      </c>
+      <c r="E139" s="18">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A132:A135"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A114:A117"/>
     <mergeCell ref="A118:A121"/>
     <mergeCell ref="A55:A58"/>
@@ -9773,18 +11062,9 @@
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="A88:A90"/>
     <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A62:A66"/>
     <mergeCell ref="A67:A71"/>
     <mergeCell ref="A72:A76"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>